<commit_message>
updated week 2 tips
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\_projects\nrl_tipping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-KKEK25T\_projects\nrl_tipping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D336A811-EDCF-474C-91EC-595F7669934A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DEFE7FBA-9B8E-43E0-898A-AAD27D11EDE2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7545" xr2:uid="{33DAC0AF-3C1A-4951-8E62-7224E491DC85}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7545" activeTab="1" xr2:uid="{33DAC0AF-3C1A-4951-8E62-7224E491DC85}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="week2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="119">
   <si>
     <t>Rocket Ryan</t>
   </si>
@@ -328,6 +329,60 @@
   </si>
   <si>
     <t>My picks</t>
+  </si>
+  <si>
+    <t>25 from 40</t>
+  </si>
+  <si>
+    <t>23 from 40</t>
+  </si>
+  <si>
+    <t>22 from 40</t>
+  </si>
+  <si>
+    <t>21 from 40</t>
+  </si>
+  <si>
+    <t>20 from 40</t>
+  </si>
+  <si>
+    <t>19 from 40</t>
+  </si>
+  <si>
+    <t>18 from 40</t>
+  </si>
+  <si>
+    <t>17 from 40</t>
+  </si>
+  <si>
+    <t>16 from 40</t>
+  </si>
+  <si>
+    <t>14 from 40</t>
+  </si>
+  <si>
+    <t>[{'Souths': 3.25, 'Syd Roosters': 1.35},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Melbourne': 1.27, 'Newcastle': 3.85},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Cronulla': 2.7, 'St George Ill': 1.48},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Brisbane': 2.7, 'Warriors': 1.47},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Bulldogs': 3.35, 'Nth Qld': 1.33},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Canberra': 1.62, 'Parramatta': 2.35},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Gold Coast': 3, 'Penrith': 1.4},</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> {'Manly': 1.67, 'Wests Tigers': 2.25}]</t>
   </si>
 </sst>
 </file>
@@ -694,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46955E31-4EC1-4E70-9A85-F98FDAB1FEFC}">
   <dimension ref="A1:AG95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AIQ34" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +1008,7 @@
         <v>32</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T3:T24" si="5">R4/R$25</f>
+        <f t="shared" ref="T4:T24" si="5">R4/R$25</f>
         <v>3.614457831325301E-2</v>
       </c>
       <c r="V4" t="s">
@@ -6349,35 +6404,35 @@
     </row>
     <row r="71" spans="1:30" x14ac:dyDescent="0.25">
       <c r="W71">
-        <f t="shared" ref="W71:W134" si="31">INDEX($I$1:$I$2,MATCH(W26,J$1:J$2,0))</f>
+        <f t="shared" ref="W71:W90" si="31">INDEX($I$1:$I$2,MATCH(W26,J$1:J$2,0))</f>
         <v>1</v>
       </c>
       <c r="X71">
-        <f t="shared" ref="X71:X134" si="32">INDEX($I$1:$I$2,MATCH(X26,K$1:K$2,0))</f>
+        <f t="shared" ref="X71:X90" si="32">INDEX($I$1:$I$2,MATCH(X26,K$1:K$2,0))</f>
         <v>1</v>
       </c>
       <c r="Y71">
-        <f t="shared" ref="Y71:Y134" si="33">INDEX($I$1:$I$2,MATCH(Y26,L$1:L$2,0))</f>
+        <f t="shared" ref="Y71:Y90" si="33">INDEX($I$1:$I$2,MATCH(Y26,L$1:L$2,0))</f>
         <v>1</v>
       </c>
       <c r="Z71">
-        <f t="shared" ref="Z71:Z134" si="34">INDEX($I$1:$I$2,MATCH(Z26,M$1:M$2,0))</f>
+        <f t="shared" ref="Z71:Z90" si="34">INDEX($I$1:$I$2,MATCH(Z26,M$1:M$2,0))</f>
         <v>1</v>
       </c>
       <c r="AA71">
-        <f t="shared" ref="AA71:AA134" si="35">INDEX($I$1:$I$2,MATCH(AA26,N$1:N$2,0))</f>
+        <f t="shared" ref="AA71:AA90" si="35">INDEX($I$1:$I$2,MATCH(AA26,N$1:N$2,0))</f>
         <v>1</v>
       </c>
       <c r="AB71">
-        <f t="shared" ref="AB71:AB134" si="36">INDEX($I$1:$I$2,MATCH(AB26,O$1:O$2,0))</f>
+        <f t="shared" ref="AB71:AB90" si="36">INDEX($I$1:$I$2,MATCH(AB26,O$1:O$2,0))</f>
         <v>2</v>
       </c>
       <c r="AC71">
-        <f t="shared" ref="AC71:AC134" si="37">INDEX($I$1:$I$2,MATCH(AC26,P$1:P$2,0))</f>
+        <f t="shared" ref="AC71:AC90" si="37">INDEX($I$1:$I$2,MATCH(AC26,P$1:P$2,0))</f>
         <v>1</v>
       </c>
       <c r="AD71">
-        <f t="shared" ref="AD71:AD134" si="38">INDEX($I$1:$I$2,MATCH(AD26,Q$1:Q$2,0))</f>
+        <f t="shared" ref="AD71:AD90" si="38">INDEX($I$1:$I$2,MATCH(AD26,Q$1:Q$2,0))</f>
         <v>1</v>
       </c>
     </row>
@@ -7173,4 +7228,1904 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{250B8CD2-AC7E-4C1B-BCE4-2B686F5643FF}">
+  <dimension ref="A2:V46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>40</v>
+      </c>
+      <c r="E2">
+        <v>0.625</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q21" si="0">VLOOKUP(H2,$A:$C,3,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ref="R2:R21" si="1">VLOOKUP(H2,$A:$D,4,FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="S2">
+        <f>Q2/R2</f>
+        <v>0.45</v>
+      </c>
+      <c r="T2">
+        <f>Q2/$Q$22</f>
+        <v>4.4009779951100246E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>0.625</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" t="s">
+        <v>68</v>
+      </c>
+      <c r="P3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S21" si="2">Q3/R3</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T21" si="3">Q3/$Q$22</f>
+        <v>5.3789731051344741E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>40</v>
+      </c>
+      <c r="E4">
+        <v>0.625</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="3"/>
+        <v>5.3789731051344741E-2</v>
+      </c>
+      <c r="V4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C5">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>0.625</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" t="s">
+        <v>61</v>
+      </c>
+      <c r="N5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O5" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="2"/>
+        <v>0.625</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>6.1124694376528114E-2</v>
+      </c>
+      <c r="V5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>40</v>
+      </c>
+      <c r="E6">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" t="s">
+        <v>72</v>
+      </c>
+      <c r="O6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P6" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>3.9119804400977995E-2</v>
+      </c>
+      <c r="V6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="E7">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>62</v>
+      </c>
+      <c r="O7" t="s">
+        <v>66</v>
+      </c>
+      <c r="P7" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>4.4009779951100246E-2</v>
+      </c>
+      <c r="V7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>40</v>
+      </c>
+      <c r="E8">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" t="s">
+        <v>61</v>
+      </c>
+      <c r="N8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O8" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="2"/>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="3"/>
+        <v>4.6454767726161368E-2</v>
+      </c>
+      <c r="V8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" t="s">
+        <v>68</v>
+      </c>
+      <c r="P9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="2"/>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="3"/>
+        <v>4.6454767726161368E-2</v>
+      </c>
+      <c r="V9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" t="s">
+        <v>72</v>
+      </c>
+      <c r="O10" t="s">
+        <v>68</v>
+      </c>
+      <c r="P10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="2"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="3"/>
+        <v>5.623471882640587E-2</v>
+      </c>
+      <c r="V10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>40</v>
+      </c>
+      <c r="E11">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" t="s">
+        <v>62</v>
+      </c>
+      <c r="O11" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="3"/>
+        <v>4.8899755501222497E-2</v>
+      </c>
+      <c r="V11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+      <c r="E12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" t="s">
+        <v>61</v>
+      </c>
+      <c r="N12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" t="s">
+        <v>68</v>
+      </c>
+      <c r="P12" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="2"/>
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="3"/>
+        <v>4.6454767726161368E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>40</v>
+      </c>
+      <c r="E13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" t="s">
+        <v>65</v>
+      </c>
+      <c r="M13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O13" t="s">
+        <v>68</v>
+      </c>
+      <c r="P13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>0.59375</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="3"/>
+        <v>4.6454767726161368E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H14" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" t="s">
+        <v>69</v>
+      </c>
+      <c r="J14" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" t="s">
+        <v>61</v>
+      </c>
+      <c r="N14" t="s">
+        <v>72</v>
+      </c>
+      <c r="O14" t="s">
+        <v>68</v>
+      </c>
+      <c r="P14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="3"/>
+        <v>5.3789731051344741E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J15" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" t="s">
+        <v>61</v>
+      </c>
+      <c r="N15" t="s">
+        <v>72</v>
+      </c>
+      <c r="O15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
+        <v>4.8899755501222497E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" t="s">
+        <v>69</v>
+      </c>
+      <c r="J16" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
+        <v>61</v>
+      </c>
+      <c r="N16" t="s">
+        <v>72</v>
+      </c>
+      <c r="O16" t="s">
+        <v>68</v>
+      </c>
+      <c r="P16" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="3"/>
+        <v>5.3789731051344741E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>40</v>
+      </c>
+      <c r="E17">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" t="s">
+        <v>63</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" t="s">
+        <v>62</v>
+      </c>
+      <c r="O17" t="s">
+        <v>68</v>
+      </c>
+      <c r="P17" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="3"/>
+        <v>5.3789731051344741E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" t="s">
+        <v>63</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" t="s">
+        <v>61</v>
+      </c>
+      <c r="N18" t="s">
+        <v>62</v>
+      </c>
+      <c r="O18" t="s">
+        <v>68</v>
+      </c>
+      <c r="P18" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>4.8899755501222497E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C19">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>40</v>
+      </c>
+      <c r="E19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" t="s">
+        <v>61</v>
+      </c>
+      <c r="N19" t="s">
+        <v>72</v>
+      </c>
+      <c r="O19" t="s">
+        <v>68</v>
+      </c>
+      <c r="P19" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>5.3789731051344741E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N20" t="s">
+        <v>72</v>
+      </c>
+      <c r="O20" t="s">
+        <v>68</v>
+      </c>
+      <c r="P20" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="2"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>5.623471882640587E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="H21" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" t="s">
+        <v>67</v>
+      </c>
+      <c r="K21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" t="s">
+        <v>65</v>
+      </c>
+      <c r="M21" t="s">
+        <v>61</v>
+      </c>
+      <c r="N21" t="s">
+        <v>72</v>
+      </c>
+      <c r="O21" t="s">
+        <v>68</v>
+      </c>
+      <c r="P21" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="S21">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>4.4009779951100246E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>0.5</v>
+      </c>
+      <c r="Q22">
+        <f>SUM(Q2:Q21)</f>
+        <v>409</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <v>0.5</v>
+      </c>
+      <c r="I23">
+        <v>3.35</v>
+      </c>
+      <c r="J23">
+        <v>2.7</v>
+      </c>
+      <c r="K23">
+        <v>3</v>
+      </c>
+      <c r="L23">
+        <v>1.62</v>
+      </c>
+      <c r="M23">
+        <v>3.25</v>
+      </c>
+      <c r="N23">
+        <v>1.67</v>
+      </c>
+      <c r="O23">
+        <v>1.27</v>
+      </c>
+      <c r="P23">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24">
+        <v>20</v>
+      </c>
+      <c r="D24">
+        <v>40</v>
+      </c>
+      <c r="E24">
+        <v>0.5</v>
+      </c>
+      <c r="I24">
+        <v>1.33</v>
+      </c>
+      <c r="J24">
+        <v>1.48</v>
+      </c>
+      <c r="K24">
+        <v>1.4</v>
+      </c>
+      <c r="L24">
+        <v>2.35</v>
+      </c>
+      <c r="M24">
+        <v>1.35</v>
+      </c>
+      <c r="N24">
+        <v>2.25</v>
+      </c>
+      <c r="O24">
+        <v>3.85</v>
+      </c>
+      <c r="P24">
+        <v>1.47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25">
+        <v>40</v>
+      </c>
+      <c r="E25">
+        <v>0.5</v>
+      </c>
+      <c r="I25">
+        <f t="shared" ref="I25:P26" si="4">1/I23</f>
+        <v>0.29850746268656714</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="4"/>
+        <v>0.37037037037037035</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="4"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="4"/>
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>0.30769230769230771</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="4"/>
+        <v>0.5988023952095809</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="4"/>
+        <v>0.78740157480314954</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>0.37037037037037035</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>40</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>0.75187969924812026</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="4"/>
+        <v>0.67567567567567566</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="4"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="4"/>
+        <v>0.42553191489361702</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>0.7407407407407407</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="4"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="4"/>
+        <v>0.25974025974025972</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>0.68027210884353739</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>40</v>
+      </c>
+      <c r="E27">
+        <v>0.5</v>
+      </c>
+      <c r="I27">
+        <f>SUM(I25:I26)</f>
+        <v>1.0503871619346874</v>
+      </c>
+      <c r="J27">
+        <f>SUM(J25:J26)</f>
+        <v>1.0460460460460461</v>
+      </c>
+      <c r="K27">
+        <f>SUM(K25:K26)</f>
+        <v>1.0476190476190477</v>
+      </c>
+      <c r="L27">
+        <f>SUM(L25:L26)</f>
+        <v>1.042815865510901</v>
+      </c>
+      <c r="M27">
+        <f>SUM(M25:M26)</f>
+        <v>1.0484330484330484</v>
+      </c>
+      <c r="N27">
+        <f>SUM(N25:N26)</f>
+        <v>1.0432468396540253</v>
+      </c>
+      <c r="O27">
+        <f>SUM(O25:O26)</f>
+        <v>1.0471418345434094</v>
+      </c>
+      <c r="P27">
+        <f>SUM(P25:P26)</f>
+        <v>1.0506424792139077</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>40</v>
+      </c>
+      <c r="E28">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" ref="I28:P29" si="5">I25-(I$27-1)/2</f>
+        <v>0.27331388171922344</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.34734734734734729</v>
+      </c>
+      <c r="K28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.30952380952380948</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.59587601786183342</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.2834757834757835</v>
+      </c>
+      <c r="N28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.57717897538256824</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.76383065753144486</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" si="5"/>
+        <v>0.34504913076341648</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29">
+        <v>19</v>
+      </c>
+      <c r="D29">
+        <v>40</v>
+      </c>
+      <c r="E29">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.72668611828077656</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.6526526526526526</v>
+      </c>
+      <c r="K29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.69047619047619047</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.40412398213816653</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.7165242165242165</v>
+      </c>
+      <c r="N29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.42282102461743176</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.23616934246855503</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" si="5"/>
+        <v>0.65495086923658352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>106</v>
+      </c>
+      <c r="C30">
+        <v>19</v>
+      </c>
+      <c r="D30">
+        <v>40</v>
+      </c>
+      <c r="E30">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="I30" t="s">
+        <v>69</v>
+      </c>
+      <c r="J30" t="s">
+        <v>57</v>
+      </c>
+      <c r="K30" t="s">
+        <v>58</v>
+      </c>
+      <c r="L30" t="s">
+        <v>60</v>
+      </c>
+      <c r="M30" t="s">
+        <v>61</v>
+      </c>
+      <c r="N30" t="s">
+        <v>72</v>
+      </c>
+      <c r="O30" t="s">
+        <v>68</v>
+      </c>
+      <c r="P30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>32</v>
+      </c>
+      <c r="E31">
+        <v>0.59375</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>40</v>
+      </c>
+      <c r="E32">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="D33">
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>106</v>
+      </c>
+      <c r="C34">
+        <v>19</v>
+      </c>
+      <c r="D34">
+        <v>40</v>
+      </c>
+      <c r="E34">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35">
+        <v>19</v>
+      </c>
+      <c r="D35">
+        <v>40</v>
+      </c>
+      <c r="E35">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36">
+        <v>19</v>
+      </c>
+      <c r="D36">
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37">
+        <v>18</v>
+      </c>
+      <c r="D37">
+        <v>40</v>
+      </c>
+      <c r="E37">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38">
+        <v>18</v>
+      </c>
+      <c r="D38">
+        <v>40</v>
+      </c>
+      <c r="E38">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39">
+        <v>18</v>
+      </c>
+      <c r="D39">
+        <v>40</v>
+      </c>
+      <c r="E39">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="D40">
+        <v>40</v>
+      </c>
+      <c r="E40">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41">
+        <v>40</v>
+      </c>
+      <c r="E41">
+        <v>0.42499999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>40</v>
+      </c>
+      <c r="E42">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>16</v>
+      </c>
+      <c r="D43">
+        <v>32</v>
+      </c>
+      <c r="E43">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44">
+        <v>14</v>
+      </c>
+      <c r="D44">
+        <v>40</v>
+      </c>
+      <c r="E44">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45">
+        <v>14</v>
+      </c>
+      <c r="D45">
+        <v>24</v>
+      </c>
+      <c r="E45">
+        <v>0.58333333333333304</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46">
+        <v>14</v>
+      </c>
+      <c r="D46">
+        <v>32</v>
+      </c>
+      <c r="E46">
+        <v>0.4375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>